<commit_message>
the files are added
</commit_message>
<xml_diff>
--- a/Framework/data/New Microsoft Excel Worksheet.xlsx
+++ b/Framework/data/New Microsoft Excel Worksheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
@@ -80,9 +80,6 @@
     <t>aagentunverified</t>
   </si>
   <si>
-    <t>TestPass2</t>
-  </si>
-  <si>
     <t>Agentban</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>userverified</t>
   </si>
   <si>
-    <t>userone</t>
-  </si>
-  <si>
     <t>userverified1@gmail.com</t>
   </si>
   <si>
@@ -132,6 +126,15 @@
   </si>
   <si>
     <t>zxcvbnm</t>
+  </si>
+  <si>
+    <t>aaadminunverified</t>
+  </si>
+  <si>
+    <t>testpass3</t>
+  </si>
+  <si>
+    <t>userone1</t>
   </si>
 </sst>
 </file>
@@ -530,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -740,7 +743,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -748,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -756,7 +759,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -764,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -772,7 +775,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -780,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -788,7 +791,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -796,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -804,7 +807,7 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -812,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -820,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="2">
-        <v>12345678</v>
+        <v>1234567890</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -828,7 +831,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -836,7 +839,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -844,7 +847,7 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -852,7 +855,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -860,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -868,7 +871,7 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -876,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -884,7 +887,7 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>